<commit_message>
period fixes + split bw + add time trends
</commit_message>
<xml_diff>
--- a/linreg/rifreg2_coefs_2.xlsx
+++ b/linreg/rifreg2_coefs_2.xlsx
@@ -258,16 +258,16 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>-0.23115182452824226</v>
+        <v>-0.23780120935333982</v>
       </c>
       <c r="C2">
-        <v>0.0071748897535214096</v>
+        <v>0.0070119080416769395</v>
       </c>
       <c r="D2">
-        <v>-0.24521438595089626</v>
+        <v>-0.2515443282740501</v>
       </c>
       <c r="E2">
-        <v>-0.21708926310558826</v>
+        <v>-0.22405809043262956</v>
       </c>
     </row>
     <row r="3">
@@ -275,16 +275,16 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>0.10869254950673425</v>
+        <v>0.11216581351611048</v>
       </c>
       <c r="C3">
-        <v>0.0027223436014140205</v>
+        <v>0.0026282775840334692</v>
       </c>
       <c r="D3">
-        <v>0.10335684046818568</v>
+        <v>0.10701447222935702</v>
       </c>
       <c r="E3">
-        <v>0.11402825854528283</v>
+        <v>0.11731715480286393</v>
       </c>
     </row>
     <row r="4">
@@ -292,16 +292,16 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>0.18997153608087966</v>
+        <v>0.20032632630161099</v>
       </c>
       <c r="C4">
-        <v>0.0096328285798122151</v>
+        <v>0.0092818499759300538</v>
       </c>
       <c r="D4">
-        <v>0.17109149077969274</v>
+        <v>0.1821341926818878</v>
       </c>
       <c r="E4">
-        <v>0.20885158138206658</v>
+        <v>0.21851845992133417</v>
       </c>
     </row>
     <row r="5">
@@ -309,16 +309,16 @@
         <v>8</v>
       </c>
       <c r="B5">
-        <v>-0.090261786383739648</v>
+        <v>-0.089584143710899664</v>
       </c>
       <c r="C5">
-        <v>0.0038680823105191882</v>
+        <v>0.0037285983220680993</v>
       </c>
       <c r="D5">
-        <v>-0.097843108108664242</v>
+        <v>-0.096892079353877753</v>
       </c>
       <c r="E5">
-        <v>-0.082680464658815053</v>
+        <v>-0.082276208067921575</v>
       </c>
     </row>
     <row r="6">
@@ -326,16 +326,16 @@
         <v>9</v>
       </c>
       <c r="B6">
-        <v>0.067064386546592608</v>
+        <v>0.068711442454373065</v>
       </c>
       <c r="C6">
-        <v>0.0023602969326978296</v>
+        <v>0.0022530516772297834</v>
       </c>
       <c r="D6">
-        <v>0.062438277540465194</v>
+        <v>0.064295531906956804</v>
       </c>
       <c r="E6">
-        <v>0.071690495552720016</v>
+        <v>0.073127353001789325</v>
       </c>
     </row>
     <row r="7">
@@ -343,16 +343,16 @@
         <v>10</v>
       </c>
       <c r="B7">
-        <v>0.065906175678553378</v>
+        <v>0.068241281570436685</v>
       </c>
       <c r="C7">
-        <v>0.0054683612236305253</v>
+        <v>0.0052427943682260003</v>
       </c>
       <c r="D7">
-        <v>0.055188356765625231</v>
+        <v>0.057965569218800909</v>
       </c>
       <c r="E7">
-        <v>0.076623994591481531</v>
+        <v>0.078516993922072453</v>
       </c>
     </row>
     <row r="8">
@@ -360,16 +360,16 @@
         <v>11</v>
       </c>
       <c r="B8">
-        <v>-0.26839087190855793</v>
+        <v>-0.26944287625901975</v>
       </c>
       <c r="C8">
-        <v>0.0061559230919704857</v>
+        <v>0.0058246516482187097</v>
       </c>
       <c r="D8">
-        <v>-0.28045629027285846</v>
+        <v>-0.28085901004134994</v>
       </c>
       <c r="E8">
-        <v>-0.2563254535442574</v>
+        <v>-0.25802674247668955</v>
       </c>
     </row>
     <row r="9">
@@ -377,16 +377,16 @@
         <v>12</v>
       </c>
       <c r="B9">
-        <v>0.2147888809700694</v>
+        <v>0.21849136632133936</v>
       </c>
       <c r="C9">
-        <v>0.0028180041687710621</v>
+        <v>0.0026502569184737508</v>
       </c>
       <c r="D9">
-        <v>0.20926568018594743</v>
+        <v>0.213296946231325</v>
       </c>
       <c r="E9">
-        <v>0.22031208175419137</v>
+        <v>0.22368578641135373</v>
       </c>
     </row>
     <row r="10">
@@ -394,16 +394,16 @@
         <v>13</v>
       </c>
       <c r="B10">
-        <v>0.16237033400632186</v>
+        <v>0.16993448992396976</v>
       </c>
       <c r="C10">
-        <v>0.0094051057120652492</v>
+        <v>0.0087939733302174906</v>
       </c>
       <c r="D10">
-        <v>0.14393661846420377</v>
+        <v>0.15269857916410334</v>
       </c>
       <c r="E10">
-        <v>0.18080404954843995</v>
+        <v>0.18717040068383617</v>
       </c>
     </row>
     <row r="11">
@@ -411,16 +411,16 @@
         <v>14</v>
       </c>
       <c r="B11">
-        <v>-0.11747990628528877</v>
+        <v>-0.11752637150882232</v>
       </c>
       <c r="C11">
-        <v>0.0038113542291632438</v>
+        <v>0.0036356244275116715</v>
       </c>
       <c r="D11">
-        <v>-0.12495004272482595</v>
+        <v>-0.12465208123760793</v>
       </c>
       <c r="E11">
-        <v>-0.1100097698457516</v>
+        <v>-0.11040066178003671</v>
       </c>
     </row>
     <row r="12">
@@ -428,16 +428,16 @@
         <v>15</v>
       </c>
       <c r="B12">
-        <v>0.11968675374823146</v>
+        <v>0.12101164159224552</v>
       </c>
       <c r="C12">
-        <v>0.0027215447669091102</v>
+        <v>0.0025790760690650185</v>
       </c>
       <c r="D12">
-        <v>0.11435261015707467</v>
+        <v>0.1159567334731489</v>
       </c>
       <c r="E12">
-        <v>0.12502089733938826</v>
+        <v>0.12606654971134215</v>
       </c>
     </row>
     <row r="13">
@@ -445,16 +445,16 @@
         <v>16</v>
       </c>
       <c r="B13">
-        <v>0.076804705482003785</v>
+        <v>0.077874113396346298</v>
       </c>
       <c r="C13">
-        <v>0.0060691195041083822</v>
+        <v>0.0057576624560337387</v>
       </c>
       <c r="D13">
-        <v>0.064909418915187006</v>
+        <v>0.066589275758124233</v>
       </c>
       <c r="E13">
-        <v>0.088699992048820564</v>
+        <v>0.089158951034568362</v>
       </c>
     </row>
     <row r="14">
@@ -462,16 +462,16 @@
         <v>17</v>
       </c>
       <c r="B14">
-        <v>-0.24280878936788181</v>
+        <v>-0.24419380014280956</v>
       </c>
       <c r="C14">
-        <v>0.005024971163683974</v>
+        <v>0.0048031904849626713</v>
       </c>
       <c r="D14">
-        <v>-0.25265757702370456</v>
+        <v>-0.2536079022162131</v>
       </c>
       <c r="E14">
-        <v>-0.23296000171205902</v>
+        <v>-0.23477969806940599</v>
       </c>
     </row>
     <row r="15">
@@ -479,16 +479,16 @@
         <v>18</v>
       </c>
       <c r="B15">
-        <v>0.27772356199890852</v>
+        <v>0.28270976582374718</v>
       </c>
       <c r="C15">
-        <v>0.0027789738961447432</v>
+        <v>0.0026393387243403362</v>
       </c>
       <c r="D15">
-        <v>0.27227685933880041</v>
+        <v>0.27753674505036435</v>
       </c>
       <c r="E15">
-        <v>0.28317026465901662</v>
+        <v>0.28788278659713001</v>
       </c>
     </row>
     <row r="16">
@@ -496,16 +496,16 @@
         <v>19</v>
       </c>
       <c r="B16">
-        <v>0.07852374375104855</v>
+        <v>0.085910302406704511</v>
       </c>
       <c r="C16">
-        <v>0.0086516763219370331</v>
+        <v>0.0081868862611263384</v>
       </c>
       <c r="D16">
-        <v>0.061566726449640105</v>
+        <v>0.069864263181968755</v>
       </c>
       <c r="E16">
-        <v>0.095480761052456994</v>
+        <v>0.10195634163144027</v>
       </c>
     </row>
     <row r="17">
@@ -513,16 +513,16 @@
         <v>20</v>
       </c>
       <c r="B17">
-        <v>-0.12035788345093378</v>
+        <v>-0.12178834401309085</v>
       </c>
       <c r="C17">
-        <v>0.0035360321418433159</v>
+        <v>0.003396818525197192</v>
       </c>
       <c r="D17">
-        <v>-0.12728839711246703</v>
+        <v>-0.12844600167122339</v>
       </c>
       <c r="E17">
-        <v>-0.11342736978940052</v>
+        <v>-0.11513068635495831</v>
       </c>
     </row>
     <row r="18">
@@ -530,16 +530,16 @@
         <v>21</v>
       </c>
       <c r="B18">
-        <v>0.16382013743685808</v>
+        <v>0.16659143793455386</v>
       </c>
       <c r="C18">
-        <v>0.0028276035365610778</v>
+        <v>0.0027103059322577706</v>
       </c>
       <c r="D18">
-        <v>0.15827812193659155</v>
+        <v>0.16127932340387532</v>
       </c>
       <c r="E18">
-        <v>0.16936215293712462</v>
+        <v>0.1719035524652324</v>
       </c>
     </row>
     <row r="19">
@@ -547,16 +547,16 @@
         <v>22</v>
       </c>
       <c r="B19">
-        <v>0.053239684112638144</v>
+        <v>0.053743469356032587</v>
       </c>
       <c r="C19">
-        <v>0.0062073620536568005</v>
+        <v>0.0059615228504391561</v>
       </c>
       <c r="D19">
-        <v>0.041073446423258594</v>
+        <v>0.042059071745461286</v>
       </c>
       <c r="E19">
-        <v>0.065405921802017694</v>
+        <v>0.065427866966603881</v>
       </c>
     </row>
     <row r="20">
@@ -564,16 +564,16 @@
         <v>23</v>
       </c>
       <c r="B20">
-        <v>-0.202552243715276</v>
+        <v>-0.20487305481564672</v>
       </c>
       <c r="C20">
-        <v>0.0042564680383484522</v>
+        <v>0.0040805792078984484</v>
       </c>
       <c r="D20">
-        <v>-0.21089478907682127</v>
+        <v>-0.21287086154474269</v>
       </c>
       <c r="E20">
-        <v>-0.19420969835373073</v>
+        <v>-0.19687524808655074</v>
       </c>
     </row>
     <row r="21">
@@ -581,16 +581,16 @@
         <v>24</v>
       </c>
       <c r="B21">
-        <v>0.29953358399508223</v>
+        <v>0.30555608605670598</v>
       </c>
       <c r="C21">
-        <v>0.0028195215012455153</v>
+        <v>0.0026877674849701736</v>
       </c>
       <c r="D21">
-        <v>0.29400740928636304</v>
+        <v>0.30028814643775892</v>
       </c>
       <c r="E21">
-        <v>0.30505975870380142</v>
+        <v>0.31082402567565304</v>
       </c>
     </row>
     <row r="22">
@@ -598,16 +598,16 @@
         <v>25</v>
       </c>
       <c r="B22">
-        <v>0.013792156170592257</v>
+        <v>0.021694275673353813</v>
       </c>
       <c r="C22">
-        <v>0.0080961460557332325</v>
+        <v>0.0077184211339620537</v>
       </c>
       <c r="D22">
-        <v>-0.0020760390361212692</v>
+        <v>0.0065664133434885572</v>
       </c>
       <c r="E22">
-        <v>0.029660351377305785</v>
+        <v>0.036822138003219068</v>
       </c>
     </row>
     <row r="23">
@@ -615,16 +615,16 @@
         <v>26</v>
       </c>
       <c r="B23">
-        <v>-0.11376622992796155</v>
+        <v>-0.1143508439081759</v>
       </c>
       <c r="C23">
-        <v>0.0033952694974970785</v>
+        <v>0.0032660070989607667</v>
       </c>
       <c r="D23">
-        <v>-0.12042085315905134</v>
+        <v>-0.12075211527802311</v>
       </c>
       <c r="E23">
-        <v>-0.10711160669687177</v>
+        <v>-0.10794957253832869</v>
       </c>
     </row>
     <row r="24">
@@ -632,16 +632,16 @@
         <v>27</v>
       </c>
       <c r="B24">
-        <v>0.1955659941820086</v>
+        <v>0.19926924539985302</v>
       </c>
       <c r="C24">
-        <v>0.003031337922465494</v>
+        <v>0.0029044336007393286</v>
       </c>
       <c r="D24">
-        <v>0.18962466558497293</v>
+        <v>0.19357664673405378</v>
       </c>
       <c r="E24">
-        <v>0.20150732277904426</v>
+        <v>0.20496184406565227</v>
       </c>
     </row>
     <row r="25">
@@ -649,16 +649,16 @@
         <v>28</v>
       </c>
       <c r="B25">
-        <v>0.04262356917150445</v>
+        <v>0.042788548428895068</v>
       </c>
       <c r="C25">
-        <v>0.0064650474014156323</v>
+        <v>0.0061878274014262862</v>
       </c>
       <c r="D25">
-        <v>0.029952276168320951</v>
+        <v>0.030660601003762437</v>
       </c>
       <c r="E25">
-        <v>0.055294862174687945</v>
+        <v>0.054916495854027698</v>
       </c>
     </row>
     <row r="26">
@@ -666,16 +666,16 @@
         <v>29</v>
       </c>
       <c r="B26">
-        <v>-0.17331113493568753</v>
+        <v>-0.17115520221954347</v>
       </c>
       <c r="C26">
-        <v>0.0039938259233301271</v>
+        <v>0.003720958722136835</v>
       </c>
       <c r="D26">
-        <v>-0.18113890989636242</v>
+        <v>-0.17844816412284173</v>
       </c>
       <c r="E26">
-        <v>-0.16548335997501265</v>
+        <v>-0.16386224031624522</v>
       </c>
     </row>
     <row r="27">
@@ -683,16 +683,16 @@
         <v>30</v>
       </c>
       <c r="B27">
-        <v>0.30662764934592401</v>
+        <v>0.30652632479985342</v>
       </c>
       <c r="C27">
-        <v>0.0031072485921276108</v>
+        <v>0.0028732812569208913</v>
       </c>
       <c r="D27">
-        <v>0.30053753846152975</v>
+        <v>0.30089478403066389</v>
       </c>
       <c r="E27">
-        <v>0.31271776023031828</v>
+        <v>0.31215786556904296</v>
       </c>
     </row>
     <row r="28">
@@ -700,16 +700,16 @@
         <v>31</v>
       </c>
       <c r="B28">
-        <v>-0.035134970672935431</v>
+        <v>-0.028759102420072236</v>
       </c>
       <c r="C28">
-        <v>0.0084043800608267355</v>
+        <v>0.0078007699643280774</v>
       </c>
       <c r="D28">
-        <v>-0.051607294971256337</v>
+        <v>-0.044048365863867532</v>
       </c>
       <c r="E28">
-        <v>-0.018662646374614521</v>
+        <v>-0.013469838976276941</v>
       </c>
     </row>
     <row r="29">
@@ -717,16 +717,16 @@
         <v>32</v>
       </c>
       <c r="B29">
-        <v>-0.11107139807208365</v>
+        <v>-0.10942786563243886</v>
       </c>
       <c r="C29">
-        <v>0.0033096138299833025</v>
+        <v>0.0031164897527257117</v>
       </c>
       <c r="D29">
-        <v>-0.11755813884337697</v>
+        <v>-0.11553608769812058</v>
       </c>
       <c r="E29">
-        <v>-0.10458465730079032</v>
+        <v>-0.10331964356675714</v>
       </c>
     </row>
     <row r="30">
@@ -734,16 +734,16 @@
         <v>33</v>
       </c>
       <c r="B30">
-        <v>0.21008760738582405</v>
+        <v>0.21057787018812663</v>
       </c>
       <c r="C30">
-        <v>0.0032594830262359102</v>
+        <v>0.0030557086130297492</v>
       </c>
       <c r="D30">
-        <v>0.20369912143979763</v>
+        <v>0.20458877724787952</v>
       </c>
       <c r="E30">
-        <v>0.21647609333185047</v>
+        <v>0.21656696312837373</v>
       </c>
     </row>
     <row r="31">
@@ -751,16 +751,16 @@
         <v>34</v>
       </c>
       <c r="B31">
-        <v>0.033949238801414684</v>
+        <v>0.032960362500908003</v>
       </c>
       <c r="C31">
-        <v>0.0068592811548863495</v>
+        <v>0.0064263377769409186</v>
       </c>
       <c r="D31">
-        <v>0.020505259831400002</v>
+        <v>0.020364942228371232</v>
       </c>
       <c r="E31">
-        <v>0.047393217771429366</v>
+        <v>0.04555578277344477</v>
       </c>
     </row>
     <row r="32">
@@ -768,16 +768,16 @@
         <v>35</v>
       </c>
       <c r="B32">
-        <v>-0.13916365745828183</v>
+        <v>-0.13817285652500857</v>
       </c>
       <c r="C32">
-        <v>0.0036699790952561639</v>
+        <v>0.0034683280441769131</v>
       </c>
       <c r="D32">
-        <v>-0.14635670267846326</v>
+        <v>-0.14497067025614219</v>
       </c>
       <c r="E32">
-        <v>-0.13197061223810039</v>
+        <v>-0.13137504279387496</v>
       </c>
     </row>
     <row r="33">
@@ -785,16 +785,16 @@
         <v>36</v>
       </c>
       <c r="B33">
-        <v>0.27172593079350743</v>
+        <v>0.27323389489622568</v>
       </c>
       <c r="C33">
-        <v>0.0032209872095532669</v>
+        <v>0.0030266646791453598</v>
       </c>
       <c r="D33">
-        <v>0.26541289574600796</v>
+        <v>0.26730172745030745</v>
       </c>
       <c r="E33">
-        <v>0.2780389658410069</v>
+        <v>0.27916606234214392</v>
       </c>
     </row>
     <row r="34">
@@ -802,16 +802,16 @@
         <v>37</v>
       </c>
       <c r="B34">
-        <v>-0.068972027600764693</v>
+        <v>-0.064929843386910976</v>
       </c>
       <c r="C34">
-        <v>0.0082554968316324064</v>
+        <v>0.007798370925615518</v>
       </c>
       <c r="D34">
-        <v>-0.085152545386752682</v>
+        <v>-0.080214404790387703</v>
       </c>
       <c r="E34">
-        <v>-0.052791509814776705</v>
+        <v>-0.049645281983434257</v>
       </c>
     </row>
     <row r="35">
@@ -819,16 +819,16 @@
         <v>38</v>
       </c>
       <c r="B35">
-        <v>-0.097972682765427976</v>
+        <v>-0.09825570228743026</v>
       </c>
       <c r="C35">
-        <v>0.0031943829632715168</v>
+        <v>0.0030590246679594976</v>
       </c>
       <c r="D35">
-        <v>-0.1042335746009817</v>
+        <v>-0.10425129459122419</v>
       </c>
       <c r="E35">
-        <v>-0.091711790929874248</v>
+        <v>-0.092260109983636332</v>
       </c>
     </row>
     <row r="36">
@@ -836,16 +836,16 @@
         <v>39</v>
       </c>
       <c r="B36">
-        <v>0.20727467679429443</v>
+        <v>0.20955131050005238</v>
       </c>
       <c r="C36">
-        <v>0.0034371652374298365</v>
+        <v>0.0032846075243989437</v>
       </c>
       <c r="D36">
-        <v>0.20053793920838076</v>
+        <v>0.20311358288035125</v>
       </c>
       <c r="E36">
-        <v>0.2140114143802081</v>
+        <v>0.21598903811975351</v>
       </c>
     </row>
     <row r="37">
@@ -853,16 +853,16 @@
         <v>40</v>
       </c>
       <c r="B37">
-        <v>0.029565833444639485</v>
+        <v>0.030426522718642064</v>
       </c>
       <c r="C37">
-        <v>0.0071949704405456869</v>
+        <v>0.0068686521207487394</v>
       </c>
       <c r="D37">
-        <v>0.015463913854469808</v>
+        <v>0.016964180219760257</v>
       </c>
       <c r="E37">
-        <v>0.043667753034809159</v>
+        <v>0.043888865217523873</v>
       </c>
     </row>
     <row r="38">
@@ -870,16 +870,16 @@
         <v>41</v>
       </c>
       <c r="B38">
-        <v>-0.10873874751511059</v>
+        <v>-0.10818951530566451</v>
       </c>
       <c r="C38">
-        <v>0.0032368695854389467</v>
+        <v>0.0030917238565077013</v>
       </c>
       <c r="D38">
-        <v>-0.11508291152683152</v>
+        <v>-0.11424919669016546</v>
       </c>
       <c r="E38">
-        <v>-0.10239458350338966</v>
+        <v>-0.10212983392116355</v>
       </c>
     </row>
     <row r="39">
@@ -887,16 +887,16 @@
         <v>42</v>
       </c>
       <c r="B39">
-        <v>0.18462882662430199</v>
+        <v>0.18707083643902572</v>
       </c>
       <c r="C39">
-        <v>0.0031092424681985042</v>
+        <v>0.0029554530354155913</v>
       </c>
       <c r="D39">
-        <v>0.17853480780463912</v>
+        <v>0.18127824157199768</v>
       </c>
       <c r="E39">
-        <v>0.19072284544396487</v>
+        <v>0.19286343130605377</v>
       </c>
     </row>
     <row r="40">
@@ -904,16 +904,16 @@
         <v>43</v>
       </c>
       <c r="B40">
-        <v>-0.074426017262083421</v>
+        <v>-0.07507097282684741</v>
       </c>
       <c r="C40">
-        <v>0.0074771469859584144</v>
+        <v>0.007118902377888362</v>
       </c>
       <c r="D40">
-        <v>-0.089080993487278548</v>
+        <v>-0.089023797276731209</v>
       </c>
       <c r="E40">
-        <v>-0.059771041036888295</v>
+        <v>-0.061118148376963617</v>
       </c>
     </row>
     <row r="41">
@@ -921,16 +921,16 @@
         <v>44</v>
       </c>
       <c r="B41">
-        <v>-0.090679044938946268</v>
+        <v>-0.089586449774134255</v>
       </c>
       <c r="C41">
-        <v>0.0033652357007265001</v>
+        <v>0.0031558678574501054</v>
       </c>
       <c r="D41">
-        <v>-0.097274802857030801</v>
+        <v>-0.095771851688705861</v>
       </c>
       <c r="E41">
-        <v>-0.084083287020861736</v>
+        <v>-0.083401047859562649</v>
       </c>
     </row>
     <row r="42">
@@ -938,16 +938,16 @@
         <v>45</v>
       </c>
       <c r="B42">
-        <v>0.19882970956052815</v>
+        <v>0.19907249746531222</v>
       </c>
       <c r="C42">
-        <v>0.0039168535724710997</v>
+        <v>0.0036711333802549326</v>
       </c>
       <c r="D42">
-        <v>0.19115279767021784</v>
+        <v>0.19187719130403844</v>
       </c>
       <c r="E42">
-        <v>0.20650662145083845</v>
+        <v>0.206267803626586</v>
       </c>
     </row>
     <row r="43">
@@ -955,16 +955,16 @@
         <v>46</v>
       </c>
       <c r="B43">
-        <v>0.022971210914879647</v>
+        <v>0.02096221083603202</v>
       </c>
       <c r="C43">
-        <v>0.0082945155198357774</v>
+        <v>0.0077484634780843279</v>
       </c>
       <c r="D43">
-        <v>0.0067142169679709034</v>
+        <v>0.0057754657005574233</v>
       </c>
       <c r="E43">
-        <v>0.039228204861788393</v>
+        <v>0.036148955971506615</v>
       </c>
     </row>
     <row r="44">
@@ -972,16 +972,16 @@
         <v>47</v>
       </c>
       <c r="B44">
-        <v>-0.099861685575095338</v>
+        <v>-0.099649642653548892</v>
       </c>
       <c r="C44">
-        <v>0.0034472089942478566</v>
+        <v>0.0032959646931615149</v>
       </c>
       <c r="D44">
-        <v>-0.10661810830542978</v>
+        <v>-0.10610962964529899</v>
       </c>
       <c r="E44">
-        <v>-0.093105262844760894</v>
+        <v>-0.093189655661798793</v>
       </c>
     </row>
     <row r="45">
@@ -989,16 +989,16 @@
         <v>48</v>
       </c>
       <c r="B45">
-        <v>0.084388350784921504</v>
+        <v>0.081373064213153878</v>
       </c>
       <c r="C45">
-        <v>0.0033890551772164717</v>
+        <v>0.0032206477266531314</v>
       </c>
       <c r="D45">
-        <v>0.07774590773261128</v>
+        <v>0.075060696103642327</v>
       </c>
       <c r="E45">
-        <v>0.091030793837231727</v>
+        <v>0.08768543232266543</v>
       </c>
     </row>
     <row r="46">
@@ -1006,16 +1006,16 @@
         <v>49</v>
       </c>
       <c r="B46">
-        <v>-0.05900465180804447</v>
+        <v>-0.059610815238342135</v>
       </c>
       <c r="C46">
-        <v>0.00752867897549514</v>
+        <v>0.0071379534919600455</v>
       </c>
       <c r="D46">
-        <v>-0.073760629134717995</v>
+        <v>-0.07360097927178906</v>
       </c>
       <c r="E46">
-        <v>-0.044248674481370945</v>
+        <v>-0.04562065120489521</v>
       </c>
     </row>
     <row r="47">
@@ -1023,16 +1023,16 @@
         <v>50</v>
       </c>
       <c r="B47">
-        <v>-0.076613024515776007</v>
+        <v>-0.077722117631489382</v>
       </c>
       <c r="C47">
-        <v>0.0035807428352943637</v>
+        <v>0.0033790285346019851</v>
       </c>
       <c r="D47">
-        <v>-0.083631169753988766</v>
+        <v>-0.084344907466614688</v>
       </c>
       <c r="E47">
-        <v>-0.069594879277563249</v>
+        <v>-0.071099327796364076</v>
       </c>
     </row>
     <row r="48">
@@ -1040,16 +1040,16 @@
         <v>51</v>
       </c>
       <c r="B48">
-        <v>0.16516941427267731</v>
+        <v>0.16393014435956857</v>
       </c>
       <c r="C48">
-        <v>0.004472984728087318</v>
+        <v>0.0042164964518062176</v>
       </c>
       <c r="D48">
-        <v>0.15640250251330665</v>
+        <v>0.1556659437010342</v>
       </c>
       <c r="E48">
-        <v>0.17393632603204798</v>
+        <v>0.17219434501810293</v>
       </c>
     </row>
     <row r="49">
@@ -1057,16 +1057,16 @@
         <v>52</v>
       </c>
       <c r="B49">
-        <v>0.00052458219329546058</v>
+        <v>0.0060801871156313777</v>
       </c>
       <c r="C49">
-        <v>0.0094767012528651617</v>
+        <v>0.0089248794825567603</v>
       </c>
       <c r="D49">
-        <v>-0.018049459236377057</v>
+        <v>-0.011412296452210872</v>
       </c>
       <c r="E49">
-        <v>0.019098623622967981</v>
+        <v>0.023572670683473625</v>
       </c>
     </row>
     <row r="50">
@@ -1074,16 +1074,16 @@
         <v>53</v>
       </c>
       <c r="B50">
-        <v>-0.095020076311002941</v>
+        <v>-0.094680740857441298</v>
       </c>
       <c r="C50">
-        <v>0.0040724189273935868</v>
+        <v>0.0039287815135156849</v>
       </c>
       <c r="D50">
-        <v>-0.10300189112246311</v>
+        <v>-0.10238102888643563</v>
       </c>
       <c r="E50">
-        <v>-0.087038261499542774</v>
+        <v>-0.086980452828446964</v>
       </c>
     </row>
     <row r="51">
@@ -1091,16 +1091,16 @@
         <v>54</v>
       </c>
       <c r="B51">
-        <v>-0.007418883363200332</v>
+        <v>-0.011733922865044511</v>
       </c>
       <c r="C51">
-        <v>0.0038125541838028069</v>
+        <v>0.0036514784695653563</v>
       </c>
       <c r="D51">
-        <v>-0.014891371335661475</v>
+        <v>-0.018890705661592466</v>
       </c>
       <c r="E51">
-        <v>5.3604609260809837e-05</v>
+        <v>-0.0045771400684965552</v>
       </c>
     </row>
     <row r="52">
@@ -1108,16 +1108,16 @@
         <v>55</v>
       </c>
       <c r="B52">
-        <v>0.0012883384250633356</v>
+        <v>-0.00014670012356988375</v>
       </c>
       <c r="C52">
-        <v>0.0081643386093564734</v>
+        <v>0.0077763052423769569</v>
       </c>
       <c r="D52">
-        <v>-0.014713512072091942</v>
+        <v>-0.015388013482860653</v>
       </c>
       <c r="E52">
-        <v>0.017290188922218612</v>
+        <v>0.015094613235720887</v>
       </c>
     </row>
     <row r="53">
@@ -1125,16 +1125,16 @@
         <v>56</v>
       </c>
       <c r="B53">
-        <v>-0.060869158231124258</v>
+        <v>-0.063111966813637427</v>
       </c>
       <c r="C53">
-        <v>0.0042907556887029213</v>
+        <v>0.0040657144072792795</v>
       </c>
       <c r="D53">
-        <v>-0.069278906707945329</v>
+        <v>-0.071080639399062451</v>
       </c>
       <c r="E53">
-        <v>-0.052459409754303188</v>
+        <v>-0.05514329422821241</v>
       </c>
     </row>
     <row r="54">
@@ -1142,16 +1142,16 @@
         <v>57</v>
       </c>
       <c r="B54">
-        <v>0.10727151667490695</v>
+        <v>0.10621357032378968</v>
       </c>
       <c r="C54">
-        <v>0.0057038592253867348</v>
+        <v>0.0053890156677009653</v>
       </c>
       <c r="D54">
-        <v>0.0960921289602924</v>
+        <v>0.095651268816150922</v>
       </c>
       <c r="E54">
-        <v>0.11845090438952149</v>
+        <v>0.11677587183142844</v>
       </c>
     </row>
     <row r="55">
@@ -1159,16 +1159,16 @@
         <v>58</v>
       </c>
       <c r="B55">
-        <v>-0.014219649737607847</v>
+        <v>-0.01036103988011374</v>
       </c>
       <c r="C55">
-        <v>0.011617570092544029</v>
+        <v>0.010980266934485139</v>
       </c>
       <c r="D55">
-        <v>-0.036989727895954061</v>
+        <v>-0.031882018319923315</v>
       </c>
       <c r="E55">
-        <v>0.0085504284207383666</v>
+        <v>0.011159938559695838</v>
       </c>
     </row>
   </sheetData>

</xml_diff>